<commit_message>
fix: Correct database import paths and add db alias for contractor services
- Fix import paths from '@/lib/neon/db' to '@/lib/neon/connection'
- Add db alias export in connection.ts for backward compatibility
- Resolve module resolution errors in contractor services
- Fix Vite build issues with missing db export
</commit_message>
<xml_diff>
--- a/docs/staff-import-ready.xlsx
+++ b/docs/staff-import-ready.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jarvis\AI Workspace\FibreFlow_React\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D665D0F-8D69-4C3E-AAB2-BCD64C40CD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E0FCCC6-83BD-48AD-BFF9-9787C1302D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A907736-6B79-42E4-A47B-1F72BA1EFEBA}"/>
   </bookViews>
@@ -22,6 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="129">
   <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
     <t>VF001</t>
   </si>
   <si>
@@ -362,9 +365,6 @@
   </si>
   <si>
     <t>start date</t>
-  </si>
-  <si>
-    <t>employee id</t>
   </si>
   <si>
     <t>name</t>
@@ -413,7 +413,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,6 +561,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFB91C1C"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -905,10 +911,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1288,12 +1295,12 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
@@ -1304,8 +1311,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>114</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>115</v>
@@ -1338,30 +1345,30 @@
         <v>124</v>
       </c>
       <c r="L1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
         <v>125</v>
@@ -1381,25 +1388,25 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
         <v>125</v>
@@ -1419,25 +1426,25 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
         <v>125</v>
@@ -1457,25 +1464,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
         <v>125</v>
@@ -1495,25 +1502,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
         <v>125</v>
@@ -1533,25 +1540,25 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
         <v>125</v>
@@ -1571,25 +1578,25 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
         <v>125</v>
@@ -1609,25 +1616,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
         <v>125</v>
@@ -1647,25 +1654,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H10" t="s">
         <v>125</v>
@@ -1685,25 +1692,25 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H11" t="s">
         <v>125</v>
@@ -1723,25 +1730,25 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>125</v>
@@ -1761,25 +1768,25 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H13" t="s">
         <v>125</v>
@@ -1799,25 +1806,25 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H14" t="s">
         <v>125</v>
@@ -1837,25 +1844,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
         <v>125</v>
@@ -1875,25 +1882,25 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H16" t="s">
         <v>125</v>
@@ -1913,25 +1920,25 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" t="s">
-        <v>49</v>
       </c>
       <c r="H17" t="s">
         <v>125</v>
@@ -1951,25 +1958,25 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
         <v>125</v>
@@ -1989,25 +1996,25 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
         <v>125</v>
@@ -2027,25 +2034,25 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
         <v>125</v>
@@ -2065,25 +2072,25 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H21" t="s">
         <v>125</v>
@@ -2103,25 +2110,25 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H22" t="s">
         <v>125</v>
@@ -2141,25 +2148,25 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H23" t="s">
         <v>125</v>
@@ -2179,25 +2186,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H24" t="s">
         <v>125</v>
@@ -2217,25 +2224,25 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H25" t="s">
         <v>125</v>
@@ -2255,25 +2262,25 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H26" t="s">
         <v>125</v>
@@ -2293,25 +2300,25 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H27" t="s">
         <v>125</v>
@@ -2331,25 +2338,25 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" t="s">
         <v>77</v>
-      </c>
-      <c r="D28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" t="s">
-        <v>76</v>
       </c>
       <c r="H28" t="s">
         <v>125</v>
@@ -2369,25 +2376,25 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H29" t="s">
         <v>125</v>

</xml_diff>